<commit_message>
Major refactoring work in process TimeZoneDataDto and TimeZoneGroupDto
</commit_message>
<xml_diff>
--- a/technicalnotes/DataStructureRelationships.xlsx
+++ b/technicalnotes/DataStructureRelationships.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoProjects\ianatzformatInfo\technicalnotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D21547-4433-4BBD-AA7A-CAE8B0FFBE64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC941C5-8808-4394-9569-E5A07B7D25FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="240" windowWidth="28230" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1410" windowWidth="28230" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zones-2Elements" sheetId="1" r:id="rId1"/>
+    <sheet name="Zones-3Elements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="49">
   <si>
     <t>2-Element Zones</t>
   </si>
@@ -144,12 +145,60 @@
   <si>
     <t>TZClass.Canonical()</t>
   </si>
+  <si>
+    <t>3-Element Time Zone</t>
+  </si>
+  <si>
+    <t>Example 'America/Argentina/Buenos_Aires'</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>America/Argentina</t>
+  </si>
+  <si>
+    <t>GroupNameValue</t>
+  </si>
+  <si>
+    <t>TypeName</t>
+  </si>
+  <si>
+    <t>IanaVariableName</t>
+  </si>
+  <si>
+    <t>americaTimeZones</t>
+  </si>
+  <si>
+    <t>FuncType</t>
+  </si>
+  <si>
+    <t>FuncName</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>TimeZoneClass</t>
+  </si>
+  <si>
+    <t>TimeZoneDeprecationStatus</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>TimeZoneGroupType</t>
+  </si>
+  <si>
+    <t>Chicago()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +215,27 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -192,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -202,6 +272,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,16 +560,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E34"/>
+  <dimension ref="A2:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="69.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -511,179 +589,761 @@
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="9"/>
+      <c r="B35" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A36" s="9"/>
+      <c r="B36" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="9"/>
+      <c r="B37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A38" s="9"/>
+      <c r="B38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A39" s="9"/>
+      <c r="B39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A40" s="9"/>
+      <c r="B40" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A42" s="9"/>
+      <c r="B42" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A43" s="9"/>
+      <c r="B43" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A44" s="9"/>
+      <c r="B44" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A45" s="9"/>
+      <c r="B45" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A46" s="9"/>
+      <c r="B46" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D51" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C52" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D53" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D54" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D55" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D56" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D57" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D58" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D59" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D60" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D61" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D62" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D63" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23AB223-6457-49FC-A52E-0CD7AB581E6F}">
+  <dimension ref="A2:E38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
+      <c r="C12" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="22" spans="2:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" t="s">
-        <v>13</v>
+      <c r="C28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>10</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E38" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored Time Zone Group and Data Dto's. Work in progress.
</commit_message>
<xml_diff>
--- a/technicalnotes/DataStructureRelationships.xlsx
+++ b/technicalnotes/DataStructureRelationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoProjects\ianatzformatInfo\technicalnotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E541DC8-7EA7-4921-B183-3DF199188A80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5101C0-E6EB-42F5-A858-FA003DB4BE7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="3165" windowWidth="28230" windowHeight="12420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="3165" windowWidth="28230" windowHeight="12420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zones-2Elements" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="89">
   <si>
     <t>2-Element Zones</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>New Time Zone Structure</t>
+  </si>
+  <si>
+    <t>TypeValue</t>
+  </si>
+  <si>
+    <t>""</t>
   </si>
 </sst>
 </file>
@@ -2078,16 +2084,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FD9DEE-1A62-43D1-8D26-CCFCD394B9C3}">
-  <dimension ref="A4:E38"/>
+  <dimension ref="A4:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -2298,7 +2304,9 @@
       <c r="C30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -2309,7 +2317,9 @@
       <c r="C31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -2320,7 +2330,9 @@
       <c r="C32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -2331,38 +2343,44 @@
       <c r="C33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2370,10 +2388,10 @@
     <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2381,16 +2399,28 @@
     <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2398,7 +2428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2055F4CB-775B-4910-980C-106580D9CA67}">
   <dimension ref="A3:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>

</xml_diff>